<commit_message>
Added OOI Bar codes where necessary for Irminger HYPM and FLMA/B
Corrected Global Irminger HYPM, FLMA/B reference designators to nominal
values, included OOI bar codes where necessary
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
@@ -160,9 +160,6 @@
     <t>37-12190</t>
   </si>
   <si>
-    <t>GI02HYPM-RIM01-00-SIOENG-000</t>
-  </si>
-  <si>
     <r>
       <t>GI02HYPM-WFP02-00-</t>
     </r>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>GI02HYPM-RIM01-02-CTDMOG039</t>
+  </si>
+  <si>
+    <t>GI02HYPM-RIM01-00-SIOENG000</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1200,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>40</v>
@@ -1337,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -1360,7 +1360,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>1</v>
@@ -1369,7 +1369,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>2</v>
@@ -1390,7 +1390,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
@@ -1399,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1">
         <v>3280</v>
@@ -1419,7 +1419,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -1428,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1">
         <v>3280</v>
@@ -1445,7 +1445,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -1454,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1">
         <v>3280</v>
@@ -1471,7 +1471,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1">
         <v>3280</v>
@@ -1497,7 +1497,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -1506,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1">
         <v>3280</v>
@@ -1526,7 +1526,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1">
         <v>3280</v>
@@ -1555,7 +1555,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1">
         <v>3280</v>
@@ -1584,7 +1584,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1">
         <v>3280</v>
@@ -1613,7 +1613,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1">
         <v>1476</v>
@@ -1642,7 +1642,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1651,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>1476</v>
@@ -1668,7 +1668,7 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1">
         <v>131</v>
@@ -1694,7 +1694,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1">
         <v>131</v>
@@ -1720,7 +1720,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1">
         <v>1109</v>
@@ -1746,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1">
         <v>1109</v>
@@ -1774,10 +1774,10 @@
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>41</v>
@@ -1800,10 +1800,10 @@
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>41</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>41</v>
@@ -1852,10 +1852,10 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>30</v>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>30</v>
@@ -1884,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
         <v>47</v>
-      </c>
-      <c r="F28" t="s">
-        <v>48</v>
       </c>
       <c r="I28" s="18"/>
     </row>

</xml_diff>

<commit_message>
Added controller UID to GI02HYPM
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
   <si>
     <t>Ref Des</t>
   </si>
@@ -168,6 +168,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>WFPENG</t>
@@ -219,6 +220,9 @@
   <si>
     <t>GI02HYPM-RIM01-00-SIOENG000</t>
   </si>
+  <si>
+    <t>OL000246</t>
+  </si>
 </sst>
 </file>
 
@@ -391,6 +395,7 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1337,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1356,7 @@
     <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="78.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
@@ -1862,6 +1867,9 @@
       </c>
       <c r="D27" s="1">
         <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Added ZPLSG to list of instruments, no cal data available
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
   <si>
     <t>Ref Des</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>KN-221-4</t>
-  </si>
-  <si>
-    <t>GI02HYPM-MFC04-01-ZPLSGA000 unit not deployed</t>
   </si>
   <si>
     <t>GI02HYPM</t>
@@ -222,6 +219,15 @@
   </si>
   <si>
     <t>OL000246</t>
+  </si>
+  <si>
+    <t>GI02HYPM-MPM01-02-ZPLSGA009</t>
+  </si>
+  <si>
+    <t>GI02HYPM-MPM01-02-ZPLSGA010</t>
+  </si>
+  <si>
+    <t>Not deployed</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1211,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -1243,10 +1249,10 @@
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>30</v>
@@ -1340,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>1</v>
@@ -1374,7 +1380,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>2</v>
@@ -1395,7 +1401,7 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
@@ -1404,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1">
         <v>3280</v>
@@ -1424,7 +1430,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
@@ -1433,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1">
         <v>3280</v>
@@ -1450,7 +1456,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -1459,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1">
         <v>3280</v>
@@ -1476,7 +1482,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -1485,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1">
         <v>3280</v>
@@ -1502,7 +1508,7 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -1511,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1">
         <v>3280</v>
@@ -1531,7 +1537,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -1540,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="1">
         <v>3280</v>
@@ -1560,7 +1566,7 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
@@ -1569,7 +1575,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1">
         <v>3280</v>
@@ -1589,7 +1595,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -1598,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1">
         <v>3280</v>
@@ -1618,7 +1624,7 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
@@ -1627,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1">
         <v>1476</v>
@@ -1647,7 +1653,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
@@ -1656,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1">
         <v>1476</v>
@@ -1673,7 +1679,7 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -1682,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1">
         <v>131</v>
@@ -1699,7 +1705,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
@@ -1708,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1">
         <v>131</v>
@@ -1725,7 +1731,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
@@ -1734,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="1">
         <v>1109</v>
@@ -1751,7 +1757,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
@@ -1760,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19" s="1">
         <v>1109</v>
@@ -1772,17 +1778,29 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
       <c r="I21" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -1790,122 +1808,131 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="1">
-        <v>59.975333333333332</v>
+      <c r="I23" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1">
+        <v>59.975333333333332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="1">
+        <v>-39.481833333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="20" t="s">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="1">
-        <v>-39.481833333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
         <v>46</v>
       </c>
-      <c r="F28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35"/>
@@ -1934,6 +1961,14 @@
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
+    </row>
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to Irminger CTDMO calibration coefficients
The following calibration coefficients added to all Irminger CTDMOs per
Redmine ticket 10208. Updates made by Rebecca Travis.

CC_wbotc
CC_a0
CC_a1
CC_a2
CC_a3
CC_ptempa0
CC_ptempa1
CC_ptempa2
CC_ptca0
CC_ptca1
CC_ptca2
CC_ptcb0
CC_ptcb1
CC_ptcb2
CC_pa0
CC_pa1
CC_pa2
CC_g
CC_h
CC_i
CC_j
CC_cpcor
CC_ctcor
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rtravis\Desktop\Cal Sheet project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="690" windowWidth="24480" windowHeight="12630" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="696" windowWidth="24480" windowHeight="12636" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="83">
   <si>
     <t>Ref Des</t>
   </si>
@@ -229,18 +229,94 @@
   <si>
     <t>Not deployed</t>
   </si>
+  <si>
+    <t>Induction ID</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>CC_wbotc</t>
+  </si>
+  <si>
+    <t>CC_a0</t>
+  </si>
+  <si>
+    <t>CC_a1</t>
+  </si>
+  <si>
+    <t>CC_a2</t>
+  </si>
+  <si>
+    <t>CC_a3</t>
+  </si>
+  <si>
+    <t>CC_ptempa0</t>
+  </si>
+  <si>
+    <t>CC_ptempa1</t>
+  </si>
+  <si>
+    <t>CC_ptempa2</t>
+  </si>
+  <si>
+    <t>CC_ptca0</t>
+  </si>
+  <si>
+    <t>CC_ptca1</t>
+  </si>
+  <si>
+    <t>CC_ptca2</t>
+  </si>
+  <si>
+    <t>CC_ptcb0</t>
+  </si>
+  <si>
+    <t>CC_ptcb1</t>
+  </si>
+  <si>
+    <t>CC_ptcb2</t>
+  </si>
+  <si>
+    <t>CC_pa0</t>
+  </si>
+  <si>
+    <t>CC_pa1</t>
+  </si>
+  <si>
+    <t>CC_pa2</t>
+  </si>
+  <si>
+    <t>CC_g</t>
+  </si>
+  <si>
+    <t>CC_h</t>
+  </si>
+  <si>
+    <t>CC_i</t>
+  </si>
+  <si>
+    <t>CC_j</t>
+  </si>
+  <si>
+    <t>CC_cpcor</t>
+  </si>
+  <si>
+    <t>CC_ctcor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,8 +503,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,7 +756,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -726,6 +828,37 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="29" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="137">
@@ -1190,26 +1323,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="10.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1380,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1291,44 +1424,44 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E6" s="13"/>
       <c r="F6" s="14"/>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
       <c r="G12" s="13"/>
@@ -1346,27 +1479,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="A52" sqref="A52:XFD56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1395,8 +1528,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1425,7 +1558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1451,7 +1584,7 @@
         <v>1.415E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1477,7 +1610,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1503,7 +1636,7 @@
         <v>7.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1532,7 +1665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1561,7 +1694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1619,7 +1752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1648,7 +1781,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1674,7 +1807,7 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1700,7 +1833,7 @@
         <v>59.975333333333332</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1726,7 +1859,7 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1752,7 +1885,7 @@
         <v>59.975333333333332</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1778,7 +1911,7 @@
         <v>-39.481833333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1795,7 +1928,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -1812,7 +1945,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1828,147 +1961,806 @@
       <c r="E25" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="30">
+        <v>39</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="31">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="27">
+        <v>1</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="32">
+        <v>59.975333329999998</v>
+      </c>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+    </row>
+    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="32">
+        <v>-39.481833330000001</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+    </row>
+    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="27">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H28" s="30">
         <v>1450</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+    </row>
+    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B29" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="27">
+        <v>1</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F29" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="1">
-        <v>59.975333333333332</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="G29" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="34">
+        <v>4.8429E-7</v>
+      </c>
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B30" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="27">
+        <v>1</v>
+      </c>
+      <c r="E30" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F30" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="1">
-        <v>-39.481833333333334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="G30" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="36">
+        <v>-1.179278E-4</v>
+      </c>
+      <c r="I30" s="35"/>
+    </row>
+    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="27">
+        <v>1</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H31" s="36">
+        <v>3.0979420000000002E-4</v>
+      </c>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="27">
+        <v>1</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="36">
+        <v>-4.6888540000000001E-6</v>
+      </c>
+      <c r="I32" s="35"/>
+    </row>
+    <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="27">
+        <v>1</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="36">
+        <v>2.0812739999999999E-7</v>
+      </c>
+      <c r="I33" s="35"/>
+    </row>
+    <row r="34" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="27">
+        <v>1</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="34">
+        <v>-69.53022</v>
+      </c>
+      <c r="I34" s="35"/>
+    </row>
+    <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="27">
+        <v>1</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="34">
+        <v>5.1155920000000001E-2</v>
+      </c>
+      <c r="I35" s="35"/>
+    </row>
+    <row r="36" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="27">
+        <v>1</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="34">
+        <v>-3.9181449999999998E-7</v>
+      </c>
+      <c r="I36" s="35"/>
+    </row>
+    <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="27">
+        <v>1</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="34">
+        <v>524720.4</v>
+      </c>
+      <c r="I37" s="35"/>
+    </row>
+    <row r="38" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="27">
+        <v>1</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" s="34">
+        <v>0.96172950000000001</v>
+      </c>
+      <c r="I38" s="35"/>
+    </row>
+    <row r="39" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="27">
+        <v>1</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" s="34">
+        <v>6.2967240000000001E-3</v>
+      </c>
+      <c r="I39" s="35"/>
+    </row>
+    <row r="40" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="27">
+        <v>1</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" s="34">
+        <v>24.981629999999999</v>
+      </c>
+      <c r="I40" s="35"/>
+    </row>
+    <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="27">
+        <v>1</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H41" s="34">
+        <v>-2.7500000000000002E-4</v>
+      </c>
+      <c r="I41" s="35"/>
+    </row>
+    <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="27">
+        <v>1</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H42" s="34">
+        <v>0</v>
+      </c>
+      <c r="I42" s="35"/>
+    </row>
+    <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="27">
+        <v>1</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" s="36">
+        <v>0.1202594</v>
+      </c>
+      <c r="I43" s="35"/>
+    </row>
+    <row r="44" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="27">
+        <v>1</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" s="36">
+        <v>4.5148339999999997E-3</v>
+      </c>
+      <c r="I44" s="35"/>
+    </row>
+    <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="27">
+        <v>1</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="36">
+        <v>-1.091899E-11</v>
+      </c>
+      <c r="I45" s="35"/>
+    </row>
+    <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="27">
+        <v>1</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H46" s="34">
+        <v>-0.98998529999999996</v>
+      </c>
+      <c r="I46" s="35"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="27">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="34">
+        <v>0.13141</v>
+      </c>
+      <c r="I47" s="35"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="27">
+        <v>1</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="H48" s="34">
+        <v>-4.18171E-4</v>
+      </c>
+      <c r="I48" s="35"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="27">
+        <v>1</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="34">
+        <v>4.723872E-5</v>
+      </c>
+      <c r="I49" s="35"/>
+    </row>
+    <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="27">
+        <v>1</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="H50" s="34">
+        <v>-9.5700000000000003E-8</v>
+      </c>
+      <c r="I50" s="35"/>
+    </row>
+    <row r="51" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="27">
+        <v>1</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="34">
+        <v>3.2499999999999998E-6</v>
+      </c>
+      <c r="I51" s="35"/>
+    </row>
+    <row r="53" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="F53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="18"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>45</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F54" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="18"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-    </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-    </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-    </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-    </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-    </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
+      <c r="I54" s="18"/>
+    </row>
+    <row r="59" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59"/>
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A60"/>
+      <c r="B60"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61"/>
+      <c r="B61"/>
+    </row>
+    <row r="62" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A62"/>
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63"/>
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A64"/>
+      <c r="B64"/>
+    </row>
+    <row r="65" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65"/>
+      <c r="B65"/>
+    </row>
+    <row r="66" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A66"/>
+      <c r="B66"/>
+    </row>
+    <row r="67" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A67"/>
+      <c r="B67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>